<commit_message>
Updated tracker and file
</commit_message>
<xml_diff>
--- a/products_new.xlsx
+++ b/products_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lalit\OneDrive\Documents\Data scrapper\Data-Scrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58EA4AB-07F9-481E-A780-0F4B176E1A1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA70B0E4-5145-437B-B351-6762407BB433}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7890" tabRatio="399" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Sku Code</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Tira</t>
   </si>
   <si>
-    <t>Blinkit</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -94,15 +91,6 @@
   </si>
   <si>
     <t>https://www.myntra.com/31420900/</t>
-  </si>
-  <si>
-    <t>https://blinkit.com/prn/m/prid/625768/</t>
-  </si>
-  <si>
-    <t>https://blinkit.com/prn/m/prid/625732/</t>
-  </si>
-  <si>
-    <t>https://blinkit.com/prn/m/prid/625762/</t>
   </si>
   <si>
     <t>https://www.tirabeauty.com/product/lamel-all-in-one-lip-tinted-plumping-oil-403-watermelon-3-ml-7608196</t>
@@ -175,7 +163,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -198,37 +186,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -240,13 +205,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -564,21 +523,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="30.140625" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="6" width="30.140625" customWidth="1"/>
-    <col min="7" max="7" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="30.140625" customWidth="1"/>
+    <col min="6" max="6" width="65.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,95 +556,80 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="F3" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E3" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D3" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C3" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G4" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E4" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="D4" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="C4" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F3" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D3" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C3" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E4" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D4" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C4" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>